<commit_message>
add data visualisation for results
</commit_message>
<xml_diff>
--- a/results_initial_run.xlsx
+++ b/results_initial_run.xlsx
@@ -954,7 +954,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1162,11 +1162,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="17214645"/>
-        <c:axId val="83444507"/>
+        <c:axId val="65003522"/>
+        <c:axId val="92120452"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="17214645"/>
+        <c:axId val="65003522"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,7 +1198,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83444507"/>
+        <c:crossAx val="92120452"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1206,7 +1206,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83444507"/>
+        <c:axId val="92120452"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1245,7 +1245,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17214645"/>
+        <c:crossAx val="65003522"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1308,9 +1308,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>344160</xdr:colOff>
+      <xdr:colOff>343800</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1319,7 +1319,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
-        <a:ext cx="8663400" cy="6286320"/>
+        <a:ext cx="8663040" cy="6285960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1367,7 +1367,7 @@
       <selection pane="topLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="80.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="12"/>

</xml_diff>